<commit_message>
\Prepare for deployment - updated project structure and configurations"
</commit_message>
<xml_diff>
--- a/src/querryRunner/user/users.xlsx
+++ b/src/querryRunner/user/users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\visha\Desktop\New folder (2)\Zopper\src\querryRunner\user\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29C91613-13A6-4303-BA95-338A28EE1766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD8EDAF-A3E2-4032-B11C-93DBBBDC4841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5124" yWindow="2736" windowWidth="17280" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
   <si>
     <t>email</t>
   </si>
@@ -37,9 +37,6 @@
     <t>region</t>
   </si>
   <si>
-    <t>assignedBrandIds</t>
-  </si>
-  <si>
     <t>assignedStoreIds</t>
   </si>
   <si>
@@ -148,36 +145,6 @@
     <t>West</t>
   </si>
   <si>
-    <t>68b2dd32cd229c0eedddf4d3, 68b2dd33cd229c0eedddf4d8</t>
-  </si>
-  <si>
-    <t>68b2dd32cd229c0eedddf4d4, 68b2dd31cd229c0eedddf4d0</t>
-  </si>
-  <si>
-    <t>68b2dd31cd229c0eedddf4d0, 68b2dd32cd229c0eedddf4d6</t>
-  </si>
-  <si>
-    <t>68b2dd33cd229c0eedddf4d7, 68b2dd32cd229c0eedddf4d5</t>
-  </si>
-  <si>
-    <t>68b2dd31cd229c0eedddf4d1, 68b2dd31cd229c0eedddf4d0</t>
-  </si>
-  <si>
-    <t>68b2dd32cd229c0eedddf4d3, 68b2dd31cd229c0eedddf4cf</t>
-  </si>
-  <si>
-    <t>68b2dd32cd229c0eedddf4d6, 68b2dd32cd229c0eedddf4d4</t>
-  </si>
-  <si>
-    <t>68b2dd32cd229c0eedddf4d2, 68b2dd32cd229c0eedddf4d5</t>
-  </si>
-  <si>
-    <t>68b2dd32cd229c0eedddf4d3, 68b2dd32cd229c0eedddf4d5</t>
-  </si>
-  <si>
-    <t>68b2dd31cd229c0eedddf4d0, 68b2dd32cd229c0eedddf4d3</t>
-  </si>
-  <si>
     <t>68b2e6e95694c33a4cf413af, 68b2e6eb5694c33a4cf413b3</t>
   </si>
   <si>
@@ -230,13 +197,31 @@
   </si>
   <si>
     <t>Vanshika Sharma</t>
+  </si>
+  <si>
+    <t>vishalshukla2043@gmail.com</t>
+  </si>
+  <si>
+    <t>test_executive</t>
+  </si>
+  <si>
+    <t>$2b$12$92t.4ukVw2l71eBvCRSN3.2d4FIhh8lcTJo97FGoEXjCLBtsvf1yK</t>
+  </si>
+  <si>
+    <t>Subham Kumar</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>68b2e6e85694c33a4cf413ab, 68b2e6e85694c33a4cf413ac, 68b2e6e95694c33a4cf413ad, 68b2e6e95694c33a4cf413ae, 68b2e6e95694c33a4cf413af, 68b2e6ea5694c33a4cf413b0, 68b2e6ea5694c33a4cf413b1, 68b2e6ea5694c33a4cf413b2, 68b2e6eb5694c33a4cf413b3, 68b2e6eb5694c33a4cf413b4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +233,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -285,16 +278,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -597,20 +593,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="6" max="6" width="32.88671875" customWidth="1"/>
-    <col min="7" max="7" width="37.6640625" customWidth="1"/>
+    <col min="6" max="6" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,271 +627,264 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
         <v>38</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
         <v>39</v>
       </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" t="s">
         <v>52</v>
       </c>
-      <c r="H2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
         <v>38</v>
       </c>
-      <c r="E3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="F12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="G12" t="s">
         <v>57</v>
       </c>
-      <c r="H7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" t="s">
-        <v>67</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A12" r:id="rId1" xr:uid="{5D4630AC-A2F1-4C06-8E4E-39553FF759A9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
correcting auth error and some visit form issue
</commit_message>
<xml_diff>
--- a/src/querryRunner/user/users.xlsx
+++ b/src/querryRunner/user/users.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\visha\Desktop\New folder (2)\Zopper\src\querryRunner\user\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\visha\Desktop\New folder (4)\Zopper\src\querryRunner\user\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691ED38D-A203-4812-96C1-239FF60A5ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2597DCF4-A9B3-42D1-9017-36C8CF51145E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="131">
   <si>
     <t>email</t>
   </si>
@@ -221,54 +221,18 @@
     <t>suvam.chatterjee@zopper.com</t>
   </si>
   <si>
-    <t>vinod.khatik@zopper.com</t>
-  </si>
-  <si>
     <t>avneesh.mishra@zopper.com</t>
   </si>
   <si>
     <t>sanjay.sonkar@zopper.com</t>
   </si>
   <si>
-    <t>Soham</t>
-  </si>
-  <si>
-    <t>Shrusti</t>
-  </si>
-  <si>
-    <t>Neeraj</t>
-  </si>
-  <si>
-    <t>Ayush</t>
-  </si>
-  <si>
-    <t>Gautam</t>
-  </si>
-  <si>
     <t>Nehal Kedia</t>
   </si>
   <si>
-    <t>Sehaj</t>
-  </si>
-  <si>
-    <t>Shubham</t>
-  </si>
-  <si>
-    <t>Shubhanshu</t>
-  </si>
-  <si>
     <t>Suvam Chatterjee</t>
   </si>
   <si>
-    <t>Vinod</t>
-  </si>
-  <si>
-    <t>Avneesh</t>
-  </si>
-  <si>
-    <t>Sanjay</t>
-  </si>
-  <si>
     <t>vikash_dubey</t>
   </si>
   <si>
@@ -371,10 +335,6 @@
     <t>store_000257, store_000258, store_000259, store_000260, store_000261, store_000262, store_000263, store_000264, store_000265, store_000266, store_000267, store_000268, store_000269, store_000270, store_000271, store_000272, store_000273, store_000274, store_000275, store_000276, store_000277, store_000278, store_000279</t>
   </si>
   <si>
-    <t>store_000280, store_000281, store_000282, store_000283, store_000284, store_000285, store_000286, store_000287, store_000288, store_000289, store_000290, store_000291]
-Suvam Chatterjee: [store_000292, store_000293, store_000294, store_000295, store_000296, store_000297</t>
-  </si>
-  <si>
     <t>store_000292, store_000293, store_000294, store_000295, store_000296, store_000297</t>
   </si>
   <si>
@@ -388,13 +348,107 @@
   </si>
   <si>
     <t>soham_patil</t>
+  </si>
+  <si>
+    <t>vinodkhatikz123@gmail.com</t>
+  </si>
+  <si>
+    <t>store_000001, store_000002, store_000003, store_000004, store_000005, store_000006, store_000007, store_000008, store_000009, store_000010,
+store_000011, store_000012, store_000013, store_000014, store_000015, store_000016, store_000017, store_000018, store_000019, store_000020,
+store_000021, store_000022, store_000023, store_000024, store_000025, store_000026, store_000027, store_000028, store_000029, store_000030,
+store_000031, store_000032, store_000033, store_000034, store_000035, store_000036, store_000037, store_000038, store_000039, store_000040,
+store_000041, store_000042, store_000043, store_000044, store_000045, store_000046, store_000047, store_000048, store_000049, store_000050,
+store_000051, store_000052, store_000053, store_000054, store_000055, store_000056, store_000057, store_000058, store_000059, store_000060,
+store_000061, store_000062, store_000063, store_000064, store_000065, store_000066, store_000067, store_000068, store_000069, store_000070,
+store_000071, store_000072, store_000073, store_000074, store_000075, store_000076, store_000077, store_000078, store_000079</t>
+  </si>
+  <si>
+    <t>user_00020</t>
+  </si>
+  <si>
+    <t>user_00021</t>
+  </si>
+  <si>
+    <t>hitesh.gaur@zopper.com</t>
+  </si>
+  <si>
+    <t>user_00022</t>
+  </si>
+  <si>
+    <t>executive_00017</t>
+  </si>
+  <si>
+    <t>executive_00018</t>
+  </si>
+  <si>
+    <t>Hitesh Gaur</t>
+  </si>
+  <si>
+    <t>hitesh_gaur</t>
+  </si>
+  <si>
+    <t>Soham Patil</t>
+  </si>
+  <si>
+    <t>Shrusti Gudmeti</t>
+  </si>
+  <si>
+    <t>Neeraj Kandwal</t>
+  </si>
+  <si>
+    <t>Ayush Joshi</t>
+  </si>
+  <si>
+    <t>Sehaj Kaushal</t>
+  </si>
+  <si>
+    <t>Shubham Gaikwad</t>
+  </si>
+  <si>
+    <t>Subhanshu Singh</t>
+  </si>
+  <si>
+    <t>Vinod Khatik</t>
+  </si>
+  <si>
+    <t>Avneesh Mishra</t>
+  </si>
+  <si>
+    <t>Sanjay Sonkar</t>
+  </si>
+  <si>
+    <t>Gautam Kumar</t>
+  </si>
+  <si>
+    <t>Rushikesh Sarode</t>
+  </si>
+  <si>
+    <t>rushikesh.sarode@zopper.com</t>
+  </si>
+  <si>
+    <t>rushikesh_sarode</t>
+  </si>
+  <si>
+    <t>Akshat Shah</t>
+  </si>
+  <si>
+    <t>akshat_shah</t>
+  </si>
+  <si>
+    <t>admin_00004</t>
+  </si>
+  <si>
+    <t>store_000280, store_000281, store_000282, store_000283, store_000284, store_000285, store_000286, store_000287, store_000288, store_000289, store_000290, store_000291</t>
+  </si>
+  <si>
+    <t>Shah.akshat1019@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,6 +481,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -479,7 +539,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -505,6 +565,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -811,23 +878,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="120" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" customWidth="1"/>
-    <col min="5" max="6" width="33.33203125" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1"/>
-    <col min="8" max="8" width="31.109375" customWidth="1"/>
-    <col min="9" max="9" width="47.109375" customWidth="1"/>
-    <col min="10" max="10" width="32.109375" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" customWidth="1"/>
+    <col min="3" max="3" width="28.88671875" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="5" max="5" width="69.77734375" customWidth="1"/>
+    <col min="6" max="7" width="33.33203125" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" customWidth="1"/>
+    <col min="9" max="9" width="31.109375" customWidth="1"/>
+    <col min="10" max="10" width="47.109375" customWidth="1"/>
     <col min="11" max="11" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -836,31 +903,31 @@
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>12</v>
@@ -871,28 +938,28 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
       <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>33</v>
       </c>
       <c r="K2">
         <v>7408108617</v>
@@ -903,28 +970,28 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>39</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>34</v>
       </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
       <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="K3">
         <v>8126005850</v>
@@ -935,25 +1002,25 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>40</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
+      <c r="I4" t="s">
+        <v>15</v>
       </c>
       <c r="K4">
         <v>8368017420</v>
@@ -964,25 +1031,25 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>48</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>32</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>21</v>
       </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" t="s">
-        <v>33</v>
+      <c r="I5" t="s">
+        <v>15</v>
       </c>
       <c r="K5">
         <v>7408108617</v>
@@ -993,25 +1060,25 @@
         <v>41</v>
       </c>
       <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>38</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>48</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>42</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>21</v>
       </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" t="s">
-        <v>43</v>
+      <c r="I6" t="s">
+        <v>15</v>
       </c>
       <c r="K6">
         <v>9990829978</v>
@@ -1022,28 +1089,28 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" t="s">
-        <v>75</v>
-      </c>
       <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s">
         <v>48</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>46</v>
       </c>
-      <c r="G7" t="s">
-        <v>9</v>
-      </c>
       <c r="H7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="J7" t="s">
-        <v>45</v>
       </c>
       <c r="K7" t="s">
         <v>47</v>
@@ -1054,29 +1121,29 @@
         <f>"user_" &amp; TEXT(ROW()-1,"00000")</f>
         <v>user_00007</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C8" t="s">
-        <v>114</v>
-      </c>
       <c r="D8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="F8" t="s">
-        <v>88</v>
-      </c>
       <c r="G8" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I8" t="s">
-        <v>101</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>62</v>
+        <v>15</v>
+      </c>
+      <c r="J8" t="s">
+        <v>89</v>
       </c>
       <c r="K8" s="5">
         <v>9821127492</v>
@@ -1087,29 +1154,29 @@
         <f>"user_" &amp; TEXT(ROW()-1,"00000")</f>
         <v>user_00008</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C9" t="s">
-        <v>76</v>
-      </c>
       <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" t="s">
-        <v>89</v>
-      </c>
       <c r="G9" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I9" t="s">
-        <v>102</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>63</v>
+        <v>15</v>
+      </c>
+      <c r="J9" t="s">
+        <v>90</v>
       </c>
       <c r="K9" s="5">
         <v>8660770668</v>
@@ -1120,29 +1187,29 @@
         <f t="shared" ref="A10:A20" si="0">"user_" &amp; TEXT(ROW()-1,"00000")</f>
         <v>user_00009</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C10" t="s">
-        <v>77</v>
-      </c>
       <c r="D10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" t="s">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
-        <v>90</v>
-      </c>
       <c r="G10" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I10" t="s">
-        <v>103</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>64</v>
+        <v>15</v>
+      </c>
+      <c r="J10" t="s">
+        <v>91</v>
       </c>
       <c r="K10" s="5">
         <v>8826300175</v>
@@ -1153,29 +1220,29 @@
         <f t="shared" si="0"/>
         <v>user_00010</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C11" t="s">
-        <v>78</v>
-      </c>
       <c r="D11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" t="s">
         <v>8</v>
       </c>
-      <c r="F11" t="s">
-        <v>91</v>
-      </c>
       <c r="G11" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I11" t="s">
-        <v>104</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>65</v>
+        <v>15</v>
+      </c>
+      <c r="J11" t="s">
+        <v>92</v>
       </c>
       <c r="K11" s="5">
         <v>8006352799</v>
@@ -1186,29 +1253,29 @@
         <f t="shared" si="0"/>
         <v>user_00011</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C12" t="s">
-        <v>79</v>
-      </c>
       <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
         <v>8</v>
       </c>
-      <c r="F12" t="s">
-        <v>92</v>
-      </c>
       <c r="G12" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>66</v>
+        <v>15</v>
+      </c>
+      <c r="J12" t="s">
+        <v>93</v>
       </c>
       <c r="K12" s="9">
         <v>8789276124</v>
@@ -1219,29 +1286,29 @@
         <f t="shared" si="0"/>
         <v>user_00012</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C13" t="s">
-        <v>80</v>
-      </c>
       <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" t="s">
         <v>8</v>
       </c>
-      <c r="F13" t="s">
-        <v>93</v>
-      </c>
       <c r="G13" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>106</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>67</v>
+        <v>15</v>
+      </c>
+      <c r="J13" t="s">
+        <v>94</v>
       </c>
       <c r="K13" s="9">
         <v>8918941003</v>
@@ -1252,29 +1319,29 @@
         <f t="shared" si="0"/>
         <v>user_00013</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C14" t="s">
-        <v>81</v>
-      </c>
       <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="F14" t="s">
-        <v>94</v>
-      </c>
       <c r="G14" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I14" t="s">
-        <v>107</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>68</v>
+        <v>15</v>
+      </c>
+      <c r="J14" t="s">
+        <v>95</v>
       </c>
       <c r="K14" s="9">
         <v>8699848784</v>
@@ -1285,62 +1352,62 @@
         <f t="shared" si="0"/>
         <v>user_00014</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C15" t="s">
-        <v>82</v>
-      </c>
       <c r="D15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" t="s">
         <v>8</v>
       </c>
-      <c r="F15" t="s">
-        <v>95</v>
-      </c>
       <c r="G15" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="H15" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I15" t="s">
-        <v>108</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>69</v>
+        <v>15</v>
+      </c>
+      <c r="J15" t="s">
+        <v>96</v>
       </c>
       <c r="K15" s="9">
         <v>9021428313</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>user_00015</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C16" t="s">
-        <v>83</v>
-      </c>
       <c r="D16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" t="s">
         <v>8</v>
       </c>
-      <c r="F16" t="s">
-        <v>96</v>
-      </c>
       <c r="G16" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>70</v>
+        <v>9</v>
+      </c>
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="K16" s="5">
         <v>8840843779</v>
@@ -1351,29 +1418,29 @@
         <f t="shared" si="0"/>
         <v>user_00016</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C17" t="s">
-        <v>84</v>
-      </c>
       <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" t="s">
         <v>8</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" t="s">
         <v>97</v>
-      </c>
-      <c r="G17" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" t="s">
-        <v>110</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="K17" s="9">
         <v>7866952866</v>
@@ -1384,29 +1451,29 @@
         <f t="shared" si="0"/>
         <v>user_00017</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" t="s">
-        <v>85</v>
+      <c r="B18" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="D18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" t="s">
         <v>8</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" t="s">
         <v>98</v>
-      </c>
-      <c r="G18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" t="s">
-        <v>111</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="K18" s="9">
         <v>9927126229</v>
@@ -1417,29 +1484,29 @@
         <f>"user_" &amp; TEXT(ROW()-1,"00000")</f>
         <v>user_00018</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" t="s">
-        <v>86</v>
+      <c r="B19" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="D19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" t="s">
         <v>8</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" t="s">
         <v>99</v>
-      </c>
-      <c r="G19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" t="s">
-        <v>112</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="K19" s="5">
         <v>7394825598</v>
@@ -1450,48 +1517,141 @@
         <f t="shared" si="0"/>
         <v>user_00019</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" t="s">
-        <v>87</v>
+      <c r="B20" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="D20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" t="s">
         <v>8</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
+        <v>88</v>
+      </c>
+      <c r="H20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" t="s">
         <v>100</v>
-      </c>
-      <c r="G20" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" t="s">
-        <v>113</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="K20" s="5">
         <v>7003388901</v>
       </c>
     </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" t="s">
+        <v>108</v>
+      </c>
+      <c r="H21" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="12">
+        <v>7862828975</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" t="s">
+        <v>125</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" s="12">
+        <v>8999311954</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>128</v>
+      </c>
+      <c r="H23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23">
+        <v>9205161581</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B9" r:id="rId3" xr:uid="{239B772D-2FFD-4B1F-BA38-4A8706D7E4BB}"/>
-    <hyperlink ref="B12" r:id="rId4" xr:uid="{EDDF45F3-706D-4D23-9CE4-09780AA61396}"/>
-    <hyperlink ref="B13" r:id="rId5" xr:uid="{1E0D4AAF-BF9C-42BF-8A54-A3BDDCCBB0B2}"/>
-    <hyperlink ref="B14" r:id="rId6" xr:uid="{CC8E45A1-DA5B-4ECD-8137-E164A32E1C75}"/>
-    <hyperlink ref="B15" r:id="rId7" xr:uid="{5CB5C11E-44E9-42C8-8548-C82B85305F6F}"/>
-    <hyperlink ref="B16" r:id="rId8" xr:uid="{DFD2C515-37FC-4DAA-9658-9147EDA5291D}"/>
-    <hyperlink ref="B17" r:id="rId9" xr:uid="{74244D8E-F745-4933-972F-5F3B1A274CD6}"/>
-    <hyperlink ref="B20" r:id="rId10" xr:uid="{AB3F31EA-92CB-4071-8920-F917D69C5AAE}"/>
-    <hyperlink ref="B19" r:id="rId11" xr:uid="{2958C183-9261-40E0-BBB3-701CE205D3D0}"/>
-    <hyperlink ref="B18" r:id="rId12" xr:uid="{6E542595-CB81-443A-9D42-6308410D171B}"/>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C12" r:id="rId3" xr:uid="{EDDF45F3-706D-4D23-9CE4-09780AA61396}"/>
+    <hyperlink ref="C13" r:id="rId4" xr:uid="{1E0D4AAF-BF9C-42BF-8A54-A3BDDCCBB0B2}"/>
+    <hyperlink ref="C14" r:id="rId5" xr:uid="{CC8E45A1-DA5B-4ECD-8137-E164A32E1C75}"/>
+    <hyperlink ref="C15" r:id="rId6" xr:uid="{5CB5C11E-44E9-42C8-8548-C82B85305F6F}"/>
+    <hyperlink ref="C16" r:id="rId7" xr:uid="{DFD2C515-37FC-4DAA-9658-9147EDA5291D}"/>
+    <hyperlink ref="C17" r:id="rId8" xr:uid="{74244D8E-F745-4933-972F-5F3B1A274CD6}"/>
+    <hyperlink ref="C20" r:id="rId9" xr:uid="{AB3F31EA-92CB-4071-8920-F917D69C5AAE}"/>
+    <hyperlink ref="C19" r:id="rId10" xr:uid="{2958C183-9261-40E0-BBB3-701CE205D3D0}"/>
+    <hyperlink ref="C18" r:id="rId11" xr:uid="{4B37E2A5-EB54-4C12-ADF0-C8B99B617794}"/>
+    <hyperlink ref="C23" r:id="rId12" xr:uid="{E0FCAE7C-AA78-4731-8E08-BB9A09C88AAA}"/>
+    <hyperlink ref="C8" r:id="rId13" xr:uid="{D5946EFD-88A6-4550-94D6-B479C2E53FA5}"/>
+    <hyperlink ref="C9" r:id="rId14" xr:uid="{210790E0-E1F6-4CFC-BE80-FEE8ED81D451}"/>
+    <hyperlink ref="C22" r:id="rId15" xr:uid="{5FEDFDDE-F063-4BFA-BFAD-F63E0EB0A0E4}"/>
+    <hyperlink ref="C21" r:id="rId16" xr:uid="{890DDDA8-B129-4DFD-B8FB-7937D5ECA484}"/>
+    <hyperlink ref="C3" r:id="rId17" xr:uid="{32B7A499-D9C4-46C2-82D5-C7B4C023B378}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>